<commit_message>
Added few new features and fixed all known bugs
Added few new features and fixed all known bugs
</commit_message>
<xml_diff>
--- a/Lib/thinBasic_Excel/Excel_Test.tbasic_2.xlsx
+++ b/Lib/thinBasic_Excel/Excel_Test.tbasic_2.xlsx
@@ -1,79 +1,5 @@
 
-<file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="153222"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\ThinBASIC_On_GitHub\ThinBASIC_On_GitHub\Lib\thinBasic_Excel\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="21285" windowHeight="11790"/>
-  </bookViews>
-  <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-  </sheets>
-  <calcPr calcId="152511"/>
-  <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
-      <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-  </extLst>
-</workbook>
-</file>
-
-<file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-  </fonts>
-  <fills count="2">
-    <fill>
-      <patternFill patternType="none"/>
-    </fill>
-    <fill>
-      <patternFill patternType="gray125"/>
-    </fill>
-  </fills>
-  <borders count="1">
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-  </borders>
-  <cellStyleXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-  </cellStyleXfs>
-  <cellXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-  </cellXfs>
-  <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
-  </cellStyles>
-  <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
-</styleSheet>
-</file>
-
-<file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=theme/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
@@ -334,14 +260,6 @@
 </a:theme>
 </file>
 
-<file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
+<file path=theme/theme/themeManager.xml><?xml version="1.0" encoding="utf-8"?>
+<a:themeManager xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main"/>
 </file>
</xml_diff>